<commit_message>
Putting the entire event together
</commit_message>
<xml_diff>
--- a/resources/data-imports/Skills/item-skills.xlsx
+++ b/resources/data-imports/Skills/item-skills.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
   <si>
     <t>name</t>
   </si>
@@ -111,6 +111,48 @@
   </si>
   <si>
     <t>As you increase this skill over time you will gain 25% towards Attack, Armour Class, Durability and Focus for a total of 200%</t>
+  </si>
+  <si>
+    <t>Clerics Prayer</t>
+  </si>
+  <si>
+    <t>Pray to your god child, pray for the light to come and heal your wounds. While training this skill, over time you will gain 2% towards your CHR for a total of 10% You will also gain 3% towards healing for an extra 15%</t>
+  </si>
+  <si>
+    <t>Clerics of War</t>
+  </si>
+  <si>
+    <t>Death comes to those who are not prepared. Raise your ac and healing by 5% per level for a total of 15% at max level</t>
+  </si>
+  <si>
+    <t>Durable Priest</t>
+  </si>
+  <si>
+    <t>Stand fast good sir! Over time raise your defense and durability by 4% for a total of 20% at max level.</t>
+  </si>
+  <si>
+    <t>Clerics Wrath</t>
+  </si>
+  <si>
+    <t>Lash out child. Lash out with the words of your god. Raise your focus and damage over time by 5% for a total of 25% at max level.</t>
+  </si>
+  <si>
+    <t>Prophets Grace</t>
+  </si>
+  <si>
+    <t>Stand in the field of battle and protect those around you and heal your wounds. Over time you will gain an additional 40% towards your Attack, 50% towards your Armour Class and 75% towards your healing.</t>
+  </si>
+  <si>
+    <t>Prophets Rage</t>
+  </si>
+  <si>
+    <t>Rage at the enemy but in a godly way. Raise your Attack and CHR by 40% and 100% at max level.</t>
+  </si>
+  <si>
+    <t>Godly Cosmic Awakening</t>
+  </si>
+  <si>
+    <t>Awaken the power of the one true god according to The Churches doctrine.</t>
   </si>
 </sst>
 </file>
@@ -450,7 +492,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,8 +500,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="25.851" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="179.242" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="257.08" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="9.283" bestFit="true" customWidth="true" style="0"/>
@@ -773,6 +815,194 @@
         <v>5</v>
       </c>
     </row>
+    <row r="10" spans="1:16">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10">
+        <v>0.02</v>
+      </c>
+      <c r="L10">
+        <v>0.03</v>
+      </c>
+      <c r="M10">
+        <v>5</v>
+      </c>
+      <c r="N10">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11">
+        <v>0.05</v>
+      </c>
+      <c r="L11">
+        <v>0.05</v>
+      </c>
+      <c r="M11">
+        <v>3</v>
+      </c>
+      <c r="N11">
+        <v>300</v>
+      </c>
+      <c r="O11" t="s">
+        <v>32</v>
+      </c>
+      <c r="P11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12">
+        <v>0.04</v>
+      </c>
+      <c r="K12">
+        <v>0.04</v>
+      </c>
+      <c r="M12">
+        <v>5</v>
+      </c>
+      <c r="N12">
+        <v>600</v>
+      </c>
+      <c r="O12" t="s">
+        <v>32</v>
+      </c>
+      <c r="P12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13">
+        <v>0.05</v>
+      </c>
+      <c r="J13">
+        <v>0.05</v>
+      </c>
+      <c r="M13">
+        <v>5</v>
+      </c>
+      <c r="N13">
+        <v>1000</v>
+      </c>
+      <c r="O13" t="s">
+        <v>32</v>
+      </c>
+      <c r="P13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="J14">
+        <v>0.08</v>
+      </c>
+      <c r="K14">
+        <v>0.1</v>
+      </c>
+      <c r="L14">
+        <v>0.15</v>
+      </c>
+      <c r="M14">
+        <v>5</v>
+      </c>
+      <c r="N14">
+        <v>1000</v>
+      </c>
+      <c r="O14" t="s">
+        <v>34</v>
+      </c>
+      <c r="P14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15">
+        <v>0.25</v>
+      </c>
+      <c r="J15">
+        <v>0.1</v>
+      </c>
+      <c r="M15">
+        <v>4</v>
+      </c>
+      <c r="N15">
+        <v>1200</v>
+      </c>
+      <c r="O15" t="s">
+        <v>38</v>
+      </c>
+      <c r="P15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16">
+        <v>0.25</v>
+      </c>
+      <c r="G16">
+        <v>0.25</v>
+      </c>
+      <c r="J16">
+        <v>0.25</v>
+      </c>
+      <c r="K16">
+        <v>0.25</v>
+      </c>
+      <c r="L16">
+        <v>0.25</v>
+      </c>
+      <c r="M16">
+        <v>5</v>
+      </c>
+      <c r="N16">
+        <v>1500</v>
+      </c>
+      <c r="O16" t="s">
+        <v>42</v>
+      </c>
+      <c r="P16">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>